<commit_message>
atualizando codigo para selenium 4.3.0
</commit_message>
<xml_diff>
--- a/aplicacao/isencao.xlsx
+++ b/aplicacao/isencao.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="4">
   <si>
     <t>pdv</t>
   </si>
@@ -30,202 +30,7 @@
     <t>Serial</t>
   </si>
   <si>
-    <t>541-361-159</t>
-  </si>
-  <si>
-    <t>541-360-944</t>
-  </si>
-  <si>
-    <t>541-557-311</t>
-  </si>
-  <si>
-    <t>541-545-025</t>
-  </si>
-  <si>
-    <t>527-600-551</t>
-  </si>
-  <si>
-    <t>527-624-558</t>
-  </si>
-  <si>
-    <t>527-624-455</t>
-  </si>
-  <si>
-    <t>6P150283</t>
-  </si>
-  <si>
-    <t>6P150498</t>
-  </si>
-  <si>
-    <t>6P150624</t>
-  </si>
-  <si>
-    <t>541-360-927</t>
-  </si>
-  <si>
-    <t>525-890-521</t>
-  </si>
-  <si>
-    <t>525-891-173</t>
-  </si>
-  <si>
-    <t>6P150131</t>
-  </si>
-  <si>
-    <t>527-624-121</t>
-  </si>
-  <si>
-    <t>527-624-366</t>
-  </si>
-  <si>
-    <t>527-601-087</t>
-  </si>
-  <si>
-    <t>541-360-894</t>
-  </si>
-  <si>
-    <t>6P150729</t>
-  </si>
-  <si>
-    <t>6P149726</t>
-  </si>
-  <si>
-    <t>527-624-501</t>
-  </si>
-  <si>
-    <t>527-624-772</t>
-  </si>
-  <si>
-    <t>6P149109</t>
-  </si>
-  <si>
-    <t>541-361-597</t>
-  </si>
-  <si>
-    <t>527-624-688</t>
-  </si>
-  <si>
-    <t>527-624-982</t>
-  </si>
-  <si>
-    <t>541-361-796</t>
-  </si>
-  <si>
-    <t>6P150801</t>
-  </si>
-  <si>
-    <t>541-374-262</t>
-  </si>
-  <si>
-    <t>541-362-069</t>
-  </si>
-  <si>
-    <t>541-373-883</t>
-  </si>
-  <si>
-    <t>541-361-653</t>
-  </si>
-  <si>
-    <t>541-373-970</t>
-  </si>
-  <si>
-    <t>541-361-120</t>
-  </si>
-  <si>
-    <t>6P149670</t>
-  </si>
-  <si>
-    <t>541-362-294</t>
-  </si>
-  <si>
-    <t>541-361-657</t>
-  </si>
-  <si>
-    <t>526-622-551</t>
-  </si>
-  <si>
-    <t>527-625-110</t>
-  </si>
-  <si>
-    <t>541-361-520</t>
-  </si>
-  <si>
-    <t>541-374-303</t>
-  </si>
-  <si>
-    <t>541-544-546</t>
-  </si>
-  <si>
-    <t>6P151069</t>
-  </si>
-  <si>
-    <t>525-891-061</t>
-  </si>
-  <si>
-    <t>541-544-799</t>
-  </si>
-  <si>
-    <t>541-557-466</t>
-  </si>
-  <si>
-    <t>541-362-193</t>
-  </si>
-  <si>
-    <t>527-624-168</t>
-  </si>
-  <si>
-    <t>527-624-184</t>
-  </si>
-  <si>
-    <t>541-557-720</t>
-  </si>
-  <si>
-    <t>526-622-562</t>
-  </si>
-  <si>
-    <t>527-600-909</t>
-  </si>
-  <si>
-    <t>541-362-215</t>
-  </si>
-  <si>
-    <t>525-890-953</t>
-  </si>
-  <si>
-    <t>526-622-358</t>
-  </si>
-  <si>
-    <t>527-270-469</t>
-  </si>
-  <si>
-    <t>541-361-492</t>
-  </si>
-  <si>
-    <t>527-624-364</t>
-  </si>
-  <si>
-    <t>6P149627</t>
-  </si>
-  <si>
-    <t>527-601-100</t>
-  </si>
-  <si>
-    <t>6P149985</t>
-  </si>
-  <si>
-    <t>527-270-312</t>
-  </si>
-  <si>
-    <t>527-600-545</t>
-  </si>
-  <si>
-    <t>526-622-685</t>
-  </si>
-  <si>
-    <t>526-622-586</t>
-  </si>
-  <si>
-    <t>6P149730</t>
+    <t>526-622-584</t>
   </si>
 </sst>
 </file>
@@ -563,8 +368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFA659"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +397,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>15264</v>
+        <v>1360</v>
       </c>
       <c r="C2" s="4">
         <v>69.900000000000006</v>
@@ -600,10 +405,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>20904</v>
+        <v>1360</v>
       </c>
       <c r="C3" s="4">
         <v>69.900000000000006</v>
@@ -611,10 +416,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>23737</v>
+        <v>1360</v>
       </c>
       <c r="C4" s="4">
         <v>69.900000000000006</v>
@@ -622,10 +427,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>25802</v>
+        <v>1360</v>
       </c>
       <c r="C5" s="4">
         <v>69.900000000000006</v>
@@ -633,10 +438,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>26965</v>
+        <v>1360</v>
       </c>
       <c r="C6" s="4">
         <v>69.900000000000006</v>
@@ -644,792 +449,272 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
-        <v>28101</v>
+        <v>1360</v>
       </c>
       <c r="C7" s="4">
-        <v>99.9</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
-        <v>28214</v>
+        <v>1360</v>
       </c>
       <c r="C8" s="4">
-        <v>24.9</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>28214</v>
+        <v>1360</v>
       </c>
       <c r="C9" s="4">
-        <v>24.9</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>28214</v>
+        <v>1360</v>
       </c>
       <c r="C10" s="4">
-        <v>24.9</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1">
-        <v>28214</v>
+        <v>1360</v>
       </c>
       <c r="C11" s="4">
-        <v>24.9</v>
+        <v>69.900000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>28731</v>
+        <v>1360</v>
       </c>
       <c r="C12" s="4">
         <v>69.900000000000006</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>29621</v>
-      </c>
-      <c r="C13" s="4">
-        <v>69.900000000000006</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
-        <v>31097</v>
-      </c>
-      <c r="C14" s="4">
-        <v>99.9</v>
-      </c>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>31670</v>
-      </c>
-      <c r="C15" s="4">
-        <v>99.9</v>
-      </c>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>33489</v>
-      </c>
-      <c r="C16" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1">
-        <v>34449</v>
-      </c>
-      <c r="C17" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1">
-        <v>34521</v>
-      </c>
-      <c r="C18" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
-        <v>34521</v>
-      </c>
-      <c r="C19" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>34914</v>
-      </c>
-      <c r="C20" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1">
-        <v>36171</v>
-      </c>
-      <c r="C21" s="4">
-        <v>79.900000000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
-        <v>41355</v>
-      </c>
-      <c r="C22" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
-        <v>41355</v>
-      </c>
-      <c r="C23" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
-        <v>41406</v>
-      </c>
-      <c r="C24" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1">
-        <v>41583</v>
-      </c>
-      <c r="C25" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>41692</v>
-      </c>
-      <c r="C26" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1">
-        <v>41747</v>
-      </c>
-      <c r="C27" s="4">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1">
-        <v>42211</v>
-      </c>
-      <c r="C28" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1">
-        <v>42275</v>
-      </c>
-      <c r="C29" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1">
-        <v>42285</v>
-      </c>
-      <c r="C30" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1">
-        <v>42351</v>
-      </c>
-      <c r="C31" s="4">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1">
-        <v>42502</v>
-      </c>
-      <c r="C32" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="1">
-        <v>42510</v>
-      </c>
-      <c r="C33" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1">
-        <v>43139</v>
-      </c>
-      <c r="C34" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="1">
-        <v>43248</v>
-      </c>
-      <c r="C35" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="1">
-        <v>43250</v>
-      </c>
-      <c r="C36" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>1470586355</v>
-      </c>
-      <c r="B37" s="1">
-        <v>43360</v>
-      </c>
-      <c r="C37" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" s="1">
-        <v>43469</v>
-      </c>
-      <c r="C38" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="1">
-        <v>44182</v>
-      </c>
-      <c r="C39" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="1">
-        <v>45034</v>
-      </c>
-      <c r="C40" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B41" s="1">
-        <v>45034</v>
-      </c>
-      <c r="C41" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="1">
-        <v>45066</v>
-      </c>
-      <c r="C42" s="4">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B43" s="1">
-        <v>46310</v>
-      </c>
-      <c r="C43" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B44" s="1">
-        <v>46400</v>
-      </c>
-      <c r="C44" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="1">
-        <v>46408</v>
-      </c>
-      <c r="C45" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>1470586397</v>
-      </c>
-      <c r="B46" s="1">
-        <v>46578</v>
-      </c>
-      <c r="C46" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1">
-        <v>46655</v>
-      </c>
-      <c r="C47" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B48" s="1">
-        <v>46696</v>
-      </c>
-      <c r="C48" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>1470586163</v>
-      </c>
-      <c r="B49" s="1">
-        <v>47221</v>
-      </c>
-      <c r="C49" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="1">
-        <v>47251</v>
-      </c>
-      <c r="C50" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51" s="1">
-        <v>47942</v>
-      </c>
-      <c r="C51" s="4">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="1">
-        <v>47953</v>
-      </c>
-      <c r="C52" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B53" s="1">
-        <v>48282</v>
-      </c>
-      <c r="C53" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
-        <v>1470586692</v>
-      </c>
-      <c r="B54" s="1">
-        <v>48517</v>
-      </c>
-      <c r="C54" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="1">
-        <v>48517</v>
-      </c>
-      <c r="C55" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
-        <v>1470586441</v>
-      </c>
-      <c r="B56" s="1">
-        <v>48557</v>
-      </c>
-      <c r="C56" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="1">
-        <v>48557</v>
-      </c>
-      <c r="C57" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B58" s="1">
-        <v>48759</v>
-      </c>
-      <c r="C58" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="1">
-        <v>48785</v>
-      </c>
-      <c r="C59" s="4">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="1">
-        <v>48796</v>
-      </c>
-      <c r="C60" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="1">
-        <v>48889</v>
-      </c>
-      <c r="C61" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>1470586898</v>
-      </c>
-      <c r="B62" s="1">
-        <v>48907</v>
-      </c>
-      <c r="C62" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>1470586299</v>
-      </c>
-      <c r="B63" s="1">
-        <v>48965</v>
-      </c>
-      <c r="C63" s="4">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="1">
-        <v>48966</v>
-      </c>
-      <c r="C64" s="4">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B65" s="1">
-        <v>49538</v>
-      </c>
-      <c r="C65" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="1">
-        <v>50246</v>
-      </c>
-      <c r="C66" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B67" s="1">
-        <v>50246</v>
-      </c>
-      <c r="C67" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>1470586022</v>
-      </c>
-      <c r="B68" s="1">
-        <v>50406</v>
-      </c>
-      <c r="C68" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
-        <v>1470586684</v>
-      </c>
-      <c r="B69" s="1">
-        <v>50406</v>
-      </c>
-      <c r="C69" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B70" s="1">
-        <v>50411</v>
-      </c>
-      <c r="C70" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="1">
-        <v>50645</v>
-      </c>
-      <c r="C71" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="1">
-        <v>50718</v>
-      </c>
-      <c r="C72" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="1">
-        <v>50718</v>
-      </c>
-      <c r="C73" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B74" s="1">
-        <v>51005</v>
-      </c>
-      <c r="C74" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="1">
-        <v>51239</v>
-      </c>
-      <c r="C75" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>1470586474</v>
-      </c>
-      <c r="B76" s="1">
-        <v>52324</v>
-      </c>
-      <c r="C76" s="4">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B77" s="1">
-        <v>52546</v>
-      </c>
-      <c r="C77" s="4">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="4"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="4"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="4"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="4"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="4"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="4"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="4"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C78" s="4"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C79" s="4"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reconfigurando e adicionando mais funcao
</commit_message>
<xml_diff>
--- a/aplicacao/isencao.xlsx
+++ b/aplicacao/isencao.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>pdv</t>
   </si>
@@ -31,132 +31,6 @@
   </si>
   <si>
     <t>Serial</t>
-  </si>
-  <si>
-    <t>6P151398</t>
-  </si>
-  <si>
-    <t>527-600-569</t>
-  </si>
-  <si>
-    <t>527-624-155</t>
-  </si>
-  <si>
-    <t>541-361-973</t>
-  </si>
-  <si>
-    <t>6P150793</t>
-  </si>
-  <si>
-    <t>527-600-963</t>
-  </si>
-  <si>
-    <t>6P150199</t>
-  </si>
-  <si>
-    <t>527-624-756</t>
-  </si>
-  <si>
-    <t>541-361-842</t>
-  </si>
-  <si>
-    <t>527-624-205</t>
-  </si>
-  <si>
-    <t>541-361-645</t>
-  </si>
-  <si>
-    <t>6P150140</t>
-  </si>
-  <si>
-    <t>6P151035</t>
-  </si>
-  <si>
-    <t>541-361-353</t>
-  </si>
-  <si>
-    <t>6P149234</t>
-  </si>
-  <si>
-    <t>527-270-447</t>
-  </si>
-  <si>
-    <t>541-361-897</t>
-  </si>
-  <si>
-    <t>541-361-331</t>
-  </si>
-  <si>
-    <t>6P150030</t>
-  </si>
-  <si>
-    <t>541-362-190</t>
-  </si>
-  <si>
-    <t>541-361-753</t>
-  </si>
-  <si>
-    <t>541-361-946</t>
-  </si>
-  <si>
-    <t>541-361-415</t>
-  </si>
-  <si>
-    <t>541-361-800</t>
-  </si>
-  <si>
-    <t>541-361-917</t>
-  </si>
-  <si>
-    <t>527-624-730</t>
-  </si>
-  <si>
-    <t>541-361-915</t>
-  </si>
-  <si>
-    <t>541-361-354</t>
-  </si>
-  <si>
-    <t>541-557-404</t>
-  </si>
-  <si>
-    <t>541-557-471</t>
-  </si>
-  <si>
-    <t>6P150003</t>
-  </si>
-  <si>
-    <t>541-361-044</t>
-  </si>
-  <si>
-    <t>6P149342</t>
-  </si>
-  <si>
-    <t>525-891-181</t>
-  </si>
-  <si>
-    <t>6P149201</t>
-  </si>
-  <si>
-    <t>6P150089</t>
-  </si>
-  <si>
-    <t>6P150525</t>
-  </si>
-  <si>
-    <t>527-600-633</t>
-  </si>
-  <si>
-    <t>6P150713</t>
-  </si>
-  <si>
-    <t>526-622-216</t>
-  </si>
-  <si>
-    <t>527-600-601</t>
-  </si>
-  <si>
-    <t>6P150130</t>
   </si>
 </sst>
 </file>
@@ -494,7 +368,7 @@
   <dimension ref="A1:XFA654"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A2" sqref="A2:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,609 +391,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>12924</v>
-      </c>
-      <c r="C2" s="1">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>13413</v>
-      </c>
-      <c r="C3" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>19646</v>
-      </c>
-      <c r="C4" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>25309</v>
-      </c>
-      <c r="C5" s="1">
-        <v>79.900000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>25309</v>
-      </c>
-      <c r="C6" s="1">
-        <v>79.900000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>28698</v>
-      </c>
-      <c r="C7" s="1">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>28990</v>
-      </c>
-      <c r="C8" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>31570</v>
-      </c>
-      <c r="C9" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>31599</v>
-      </c>
-      <c r="C10" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1470586905</v>
-      </c>
-      <c r="B11" s="1">
-        <v>35565</v>
-      </c>
-      <c r="C11" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>38865</v>
-      </c>
-      <c r="C12" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>40304</v>
-      </c>
-      <c r="C13" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="1">
-        <v>40822</v>
-      </c>
-      <c r="C14" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="1">
-        <v>40931</v>
-      </c>
-      <c r="C15" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>41415</v>
-      </c>
-      <c r="C16" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="1">
-        <v>41494</v>
-      </c>
-      <c r="C17" s="1">
-        <v>79.900000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1">
-        <v>42575</v>
-      </c>
-      <c r="C18" s="1">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="1">
-        <v>43396</v>
-      </c>
-      <c r="C19" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="1">
-        <v>43422</v>
-      </c>
-      <c r="C20" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1">
-        <v>43797</v>
-      </c>
-      <c r="C21" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="1">
-        <v>44072</v>
-      </c>
-      <c r="C22" s="1">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="1">
-        <v>44343</v>
-      </c>
-      <c r="C23" s="1">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1">
-        <v>44496</v>
-      </c>
-      <c r="C24" s="1">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="1">
-        <v>44563</v>
-      </c>
-      <c r="C25" s="1">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="1">
-        <v>44596</v>
-      </c>
-      <c r="C26" s="1">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1">
-        <v>44756</v>
-      </c>
-      <c r="C27" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="1">
-        <v>44938</v>
-      </c>
-      <c r="C28" s="1">
-        <v>59.9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1">
-        <v>46225</v>
-      </c>
-      <c r="C29" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="1">
-        <v>46482</v>
-      </c>
-      <c r="C30" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>1470586472</v>
-      </c>
-      <c r="B31" s="1">
-        <v>46838</v>
-      </c>
-      <c r="C31" s="1">
-        <v>24.9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1">
-        <v>47157</v>
-      </c>
-      <c r="C32" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1">
-        <v>47712</v>
-      </c>
-      <c r="C33" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1">
-        <v>47811</v>
-      </c>
-      <c r="C34" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>1470586382</v>
-      </c>
-      <c r="B35" s="1">
-        <v>47962</v>
-      </c>
-      <c r="C35" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>1470586974</v>
-      </c>
-      <c r="B36" s="1">
-        <v>48168</v>
-      </c>
-      <c r="C36" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37" s="1">
-        <v>48899</v>
-      </c>
-      <c r="C37" s="1">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="1">
-        <v>48912</v>
-      </c>
-      <c r="C38" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>1470586402</v>
-      </c>
-      <c r="B39" s="1">
-        <v>48961</v>
-      </c>
-      <c r="C39" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="1">
-        <v>49564</v>
-      </c>
-      <c r="C40" s="1">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>1470586924</v>
-      </c>
-      <c r="B41" s="1">
-        <v>49568</v>
-      </c>
-      <c r="C41" s="1">
-        <v>9.9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="1">
-        <v>49896</v>
-      </c>
-      <c r="C42" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B43" s="1">
-        <v>49896</v>
-      </c>
-      <c r="C43" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="1">
-        <v>49896</v>
-      </c>
-      <c r="C44" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="1">
-        <v>50460</v>
-      </c>
-      <c r="C45" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>1470586589</v>
-      </c>
-      <c r="B46" s="1">
-        <v>50923</v>
-      </c>
-      <c r="C46" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B47" s="1">
-        <v>51131</v>
-      </c>
-      <c r="C47" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="1">
-        <v>51281</v>
-      </c>
-      <c r="C48" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="1">
-        <v>51297</v>
-      </c>
-      <c r="C49" s="1">
-        <v>69.900000000000006</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
-        <v>1470586437</v>
-      </c>
-      <c r="B50" s="1">
-        <v>51731</v>
-      </c>
-      <c r="C50" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="1">
-        <v>52264</v>
-      </c>
-      <c r="C51" s="1">
-        <v>99.9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
-        <v>1470586023</v>
-      </c>
-      <c r="B52" s="1">
-        <v>52892</v>
-      </c>
-      <c r="C52" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>1470586135</v>
-      </c>
-      <c r="B53" s="1">
-        <v>53580</v>
-      </c>
-      <c r="C53" s="1">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="3"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="3"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="3"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="3"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="3"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="3"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="3"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>